<commit_message>
danh gia phan tram lam cua ban than
</commit_message>
<xml_diff>
--- a/document/java-project-2013-bang_diem.xlsx
+++ b/document/java-project-2013-bang_diem.xlsx
@@ -1037,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1137,6 +1137,60 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1146,59 +1200,11 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -1514,20 +1520,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="34"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
       <c r="A3" t="s">
@@ -1536,10 +1542,10 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" t="s">
@@ -1548,10 +1554,10 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" t="s">
@@ -1560,22 +1566,22 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="55"/>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1">
       <c r="A7" t="s">
@@ -1584,18 +1590,18 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="42"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1">
       <c r="A9" s="8" t="s">
@@ -1619,11 +1625,11 @@
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1">
       <c r="B12" s="17"/>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="36" t="s">
         <v>245</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
     </row>
     <row r="13" spans="1:5" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B13" s="17"/>
@@ -1648,8 +1654,12 @@
       <c r="C15" s="31">
         <v>1</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
+      <c r="D15" s="31">
+        <v>1012356</v>
+      </c>
+      <c r="E15" s="31">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B16" s="17"/>
@@ -1669,29 +1679,29 @@
     </row>
     <row r="18" spans="1:6" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B18" s="17"/>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="D18" s="45"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="41"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="46"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1">
       <c r="A22" s="18" t="s">
@@ -1771,11 +1781,11 @@
       <c r="A27" s="18">
         <v>4</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="50"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
     </row>
@@ -1845,11 +1855,11 @@
       <c r="A33" s="18">
         <v>6</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
     </row>
@@ -1893,11 +1903,11 @@
       <c r="A37" s="18">
         <v>7</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="23"/>
       <c r="F37" s="23"/>
     </row>
@@ -1955,11 +1965,11 @@
       <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A42" s="53" t="s">
+      <c r="A42" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="51"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
       <c r="F42" s="23"/>
@@ -2060,12 +2070,12 @@
       <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="46"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="48"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="23"/>
       <c r="F50" s="23"/>
     </row>
@@ -2220,12 +2230,12 @@
       <c r="F61" s="23"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="46"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="48"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="23"/>
       <c r="F62" s="23"/>
     </row>
@@ -2296,12 +2306,12 @@
       <c r="F67" s="23"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="46"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="46"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="33"/>
       <c r="E68" s="23"/>
       <c r="F68" s="23"/>
     </row>
@@ -2398,12 +2408,12 @@
       <c r="F75" s="23"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="46" t="s">
+      <c r="A76" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="46"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="46"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="23"/>
       <c r="F76" s="23"/>
     </row>
@@ -2613,6 +2623,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A76:D76"/>
@@ -2622,17 +2643,6 @@
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A50:D50"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>